<commit_message>
add group and pertanyaan
</commit_message>
<xml_diff>
--- a/assets/download/mahasiswa.xlsx
+++ b/assets/download/mahasiswa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kuesioner\assets\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63B49AD-B8F4-4620-92E8-124A8D135FB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC162960-6A77-47B8-868D-E5E31EB70518}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Ana Suryaningsih</t>
   </si>
@@ -35,17 +35,26 @@
   </si>
   <si>
     <t>Angkatan</t>
+  </si>
+  <si>
+    <t>Prodi ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,19 +384,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -394,21 +405,27 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>67423747</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
+        <v>13201</v>
+      </c>
+      <c r="D2">
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>18922633</v>
       </c>
@@ -416,11 +433,15 @@
         <v>0</v>
       </c>
       <c r="C3">
+        <v>14001</v>
+      </c>
+      <c r="D3">
         <v>2017</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>